<commit_message>
Updated IC Conditions & 2D fvc files
</commit_message>
<xml_diff>
--- a/matlab/initial_conditions/create_initial_conditions/Defaults_2013_HN.xlsx
+++ b/matlab/initial_conditions/create_initial_conditions/Defaults_2013_HN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Hawkesbury\matlab\initial_conditions\create_initial_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37528248-AE4D-43C3-B8B7-597A9D090F4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48942DC-A4C2-4B45-8566-57E37209D549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="1980" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="4110" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mean_Initial_Condition" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Zone 3</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>WQ_TRC_AGE</t>
+  </si>
+  <si>
+    <t>SAL</t>
+  </si>
+  <si>
+    <t>TEMP</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1081,443 +1087,455 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4">
-        <v>10.4</v>
-      </c>
-      <c r="C3" s="4">
-        <v>10.4</v>
-      </c>
-      <c r="D3" s="4">
-        <v>10.4</v>
-      </c>
-      <c r="E3" s="4">
-        <v>10.4</v>
-      </c>
-      <c r="F3" s="4">
-        <v>10.4</v>
-      </c>
-      <c r="G3" s="4">
-        <v>10.4</v>
-      </c>
-      <c r="H3" s="4">
-        <v>10.4</v>
-      </c>
-      <c r="I3" s="4">
-        <v>10.4</v>
-      </c>
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4">
-        <v>301.875</v>
-      </c>
-      <c r="C4" s="4">
-        <v>301.875</v>
-      </c>
-      <c r="D4" s="4">
-        <v>301.875</v>
-      </c>
-      <c r="E4" s="4">
-        <v>301.875</v>
-      </c>
-      <c r="F4" s="4">
-        <v>301.875</v>
-      </c>
-      <c r="G4" s="4">
-        <v>301.875</v>
-      </c>
-      <c r="H4" s="4">
-        <v>301.875</v>
-      </c>
-      <c r="I4" s="4">
-        <v>301.875</v>
-      </c>
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5">
+        <v>12</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4">
-        <v>254.80430000000001</v>
+        <v>10.4</v>
       </c>
       <c r="C5" s="4">
-        <v>254.80430000000001</v>
+        <v>10.4</v>
       </c>
       <c r="D5" s="4">
-        <v>254.80430000000001</v>
+        <v>10.4</v>
       </c>
       <c r="E5" s="4">
-        <v>254.80430000000001</v>
+        <v>10.4</v>
       </c>
       <c r="F5" s="4">
-        <v>645.64059999999995</v>
+        <v>10.4</v>
       </c>
       <c r="G5" s="4">
-        <v>59.573</v>
+        <v>10.4</v>
       </c>
       <c r="H5" s="4">
-        <v>59.573</v>
+        <v>10.4</v>
       </c>
       <c r="I5" s="4">
-        <v>59.573</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4">
-        <v>0.53569999999999995</v>
+        <v>301.875</v>
       </c>
       <c r="C6" s="4">
-        <v>0.71430000000000005</v>
+        <v>301.875</v>
       </c>
       <c r="D6" s="4">
-        <v>1.6875</v>
+        <v>301.875</v>
       </c>
       <c r="E6" s="4">
-        <v>1.3163</v>
+        <v>301.875</v>
       </c>
       <c r="F6" s="4">
-        <v>1.3163</v>
+        <v>301.875</v>
       </c>
       <c r="G6" s="4">
-        <v>0.56169999999999998</v>
+        <v>301.875</v>
       </c>
       <c r="H6" s="4">
-        <v>6.5102000000000002</v>
+        <v>301.875</v>
       </c>
       <c r="I6" s="4">
-        <v>12</v>
+        <v>301.875</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="4">
-        <v>3.9285999999999999</v>
+        <v>254.80430000000001</v>
       </c>
       <c r="C7" s="4">
-        <v>1.4286000000000001</v>
+        <v>254.80430000000001</v>
       </c>
       <c r="D7" s="4">
-        <v>7.3392999999999997</v>
+        <v>254.80430000000001</v>
       </c>
       <c r="E7" s="4">
-        <v>23.839300000000001</v>
+        <v>254.80430000000001</v>
       </c>
       <c r="F7" s="4">
-        <v>23.839300000000001</v>
+        <v>645.64059999999995</v>
       </c>
       <c r="G7" s="4">
-        <v>19.601099999999999</v>
+        <v>59.573</v>
       </c>
       <c r="H7" s="4">
-        <v>18.571400000000001</v>
+        <v>59.573</v>
       </c>
       <c r="I7" s="4">
-        <v>123.8571</v>
+        <v>59.573</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4">
-        <v>0.3972</v>
+        <v>0.53569999999999995</v>
       </c>
       <c r="C8" s="4">
-        <v>0.3972</v>
+        <v>0.71430000000000005</v>
       </c>
       <c r="D8" s="4">
-        <v>0.3972</v>
+        <v>1.6875</v>
       </c>
       <c r="E8" s="4">
-        <v>0.2893</v>
+        <v>1.3163</v>
       </c>
       <c r="F8" s="4">
-        <v>0.2893</v>
+        <v>1.3163</v>
       </c>
       <c r="G8" s="4">
-        <v>0.16059999999999999</v>
+        <v>0.56169999999999998</v>
       </c>
       <c r="H8" s="4">
-        <v>0.18060000000000001</v>
+        <v>6.5102000000000002</v>
       </c>
       <c r="I8" s="4">
-        <v>2.4355000000000002</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4">
-        <v>3.9720000000000005E-2</v>
+        <v>3.9285999999999999</v>
       </c>
       <c r="C9" s="4">
-        <v>3.9720000000000005E-2</v>
+        <v>1.4286000000000001</v>
       </c>
       <c r="D9" s="4">
-        <v>3.9720000000000005E-2</v>
+        <v>7.3392999999999997</v>
       </c>
       <c r="E9" s="4">
-        <v>2.8930000000000001E-2</v>
+        <v>23.839300000000001</v>
       </c>
       <c r="F9" s="4">
-        <v>2.8930000000000001E-2</v>
+        <v>23.839300000000001</v>
       </c>
       <c r="G9" s="4">
-        <v>1.6060000000000001E-2</v>
+        <v>19.601099999999999</v>
       </c>
       <c r="H9" s="4">
-        <v>1.8060000000000003E-2</v>
+        <v>18.571400000000001</v>
       </c>
       <c r="I9" s="4">
-        <v>0.24355000000000004</v>
+        <v>123.8571</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4">
-        <v>104.16666666666667</v>
+        <v>0.3972</v>
       </c>
       <c r="C10" s="4">
-        <v>208.33333333333334</v>
+        <v>0.3972</v>
       </c>
       <c r="D10" s="4">
-        <v>208.33333333333334</v>
+        <v>0.3972</v>
       </c>
       <c r="E10" s="4">
-        <v>208.33333333333334</v>
+        <v>0.2893</v>
       </c>
       <c r="F10" s="4">
-        <v>208.33333333333334</v>
+        <v>0.2893</v>
       </c>
       <c r="G10" s="4">
-        <v>208.33333333333334</v>
+        <v>0.16059999999999999</v>
       </c>
       <c r="H10" s="4">
-        <v>208.33333333333334</v>
+        <v>0.18060000000000001</v>
       </c>
       <c r="I10" s="4">
-        <v>416.66666666666669</v>
+        <v>2.4355000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="4">
-        <v>104.16666666666667</v>
+        <v>3.9720000000000005E-2</v>
       </c>
       <c r="C11" s="4">
-        <v>208.33333333333334</v>
+        <v>3.9720000000000005E-2</v>
       </c>
       <c r="D11" s="4">
-        <v>208.33333333333334</v>
+        <v>3.9720000000000005E-2</v>
       </c>
       <c r="E11" s="4">
-        <v>208.33333333333334</v>
+        <v>2.8930000000000001E-2</v>
       </c>
       <c r="F11" s="4">
-        <v>208.33333333333334</v>
+        <v>2.8930000000000001E-2</v>
       </c>
       <c r="G11" s="4">
-        <v>208.33333333333334</v>
+        <v>1.6060000000000001E-2</v>
       </c>
       <c r="H11" s="4">
-        <v>208.33333333333334</v>
+        <v>1.8060000000000003E-2</v>
       </c>
       <c r="I11" s="4">
-        <v>416.66666666666669</v>
+        <v>0.24355000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="4">
-        <v>7.4106999999999994</v>
+        <v>104.16666666666667</v>
       </c>
       <c r="C12" s="4">
-        <v>5.7142499999999998</v>
+        <v>208.33333333333334</v>
       </c>
       <c r="D12" s="4">
-        <v>10.946400000000001</v>
+        <v>208.33333333333334</v>
       </c>
       <c r="E12" s="4">
-        <v>12.868649999999999</v>
+        <v>208.33333333333334</v>
       </c>
       <c r="F12" s="4">
-        <v>12.868649999999999</v>
+        <v>208.33333333333334</v>
       </c>
       <c r="G12" s="4">
-        <v>9.1123000000000012</v>
+        <v>208.33333333333334</v>
       </c>
       <c r="H12" s="4">
-        <v>6.3448999999999991</v>
+        <v>208.33333333333334</v>
       </c>
       <c r="I12" s="4">
-        <v>32.357150000000004</v>
+        <v>416.66666666666669</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4">
+        <v>104.16666666666667</v>
+      </c>
+      <c r="C13" s="4">
+        <v>208.33333333333334</v>
+      </c>
+      <c r="D13" s="4">
+        <v>208.33333333333334</v>
+      </c>
+      <c r="E13" s="4">
+        <v>208.33333333333334</v>
+      </c>
+      <c r="F13" s="4">
+        <v>208.33333333333334</v>
+      </c>
+      <c r="G13" s="4">
+        <v>208.33333333333334</v>
+      </c>
+      <c r="H13" s="4">
+        <v>208.33333333333334</v>
+      </c>
+      <c r="I13" s="4">
+        <v>416.66666666666669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4">
         <v>7.4106999999999994</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>5.7142499999999998</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D14" s="4">
         <v>10.946400000000001</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E14" s="4">
         <v>12.868649999999999</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F14" s="4">
         <v>12.868649999999999</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G14" s="4">
         <v>9.1123000000000012</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H14" s="4">
         <v>6.3448999999999991</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I14" s="4">
         <v>32.357150000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0.10414</v>
-      </c>
-      <c r="C14" s="4">
-        <v>8.7989999999999999E-2</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.21773999999999999</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0.36788500000000002</v>
-      </c>
-      <c r="F14" s="4">
-        <v>0.36788500000000002</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0.14347000000000001</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0.14391999999999996</v>
-      </c>
-      <c r="I14" s="4">
-        <v>1.2314249999999998</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="4">
+        <v>7.4106999999999994</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5.7142499999999998</v>
+      </c>
+      <c r="D15" s="4">
+        <v>10.946400000000001</v>
+      </c>
+      <c r="E15" s="4">
+        <v>12.868649999999999</v>
+      </c>
+      <c r="F15" s="4">
+        <v>12.868649999999999</v>
+      </c>
+      <c r="G15" s="4">
+        <v>9.1123000000000012</v>
+      </c>
+      <c r="H15" s="4">
+        <v>6.3448999999999991</v>
+      </c>
+      <c r="I15" s="4">
+        <v>32.357150000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4">
         <v>0.10414</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C16" s="4">
         <v>8.7989999999999999E-2</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D16" s="4">
         <v>0.21773999999999999</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E16" s="4">
         <v>0.36788500000000002</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F16" s="4">
         <v>0.36788500000000002</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G16" s="4">
         <v>0.14347000000000001</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H16" s="4">
         <v>0.14391999999999996</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I16" s="4">
         <v>1.2314249999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>9.5625</v>
-      </c>
-      <c r="E16" s="4">
-        <v>19.576354166666668</v>
-      </c>
-      <c r="F16" s="4">
-        <v>19.576354166666668</v>
-      </c>
-      <c r="G16" s="4">
-        <v>6.4210416666666674</v>
-      </c>
-      <c r="H16" s="4">
-        <v>2.0277777777777781</v>
-      </c>
-      <c r="I16" s="4">
-        <v>8.4722222222222232</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="4">
-        <v>4.4247916666666667</v>
+        <v>0.10414</v>
       </c>
       <c r="C17" s="4">
-        <v>4.4247916666666667</v>
+        <v>8.7989999999999999E-2</v>
       </c>
       <c r="D17" s="4">
-        <v>9.5625</v>
+        <v>0.21773999999999999</v>
       </c>
       <c r="E17" s="4">
-        <v>19.576354166666668</v>
+        <v>0.36788500000000002</v>
       </c>
       <c r="F17" s="4">
-        <v>19.576354166666668</v>
+        <v>0.36788500000000002</v>
       </c>
       <c r="G17" s="4">
-        <v>6.4210416666666674</v>
+        <v>0.14347000000000001</v>
       </c>
       <c r="H17" s="4">
-        <v>2.0277777777777781</v>
+        <v>0.14391999999999996</v>
       </c>
       <c r="I17" s="4">
-        <v>8.4722222222222232</v>
+        <v>1.2314249999999998</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="4">
         <v>0</v>
@@ -1546,7 +1564,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="4">
         <v>4.4247916666666667</v>
@@ -1567,15 +1585,15 @@
         <v>6.4210416666666674</v>
       </c>
       <c r="H19" s="4">
-        <v>0</v>
+        <v>2.0277777777777781</v>
       </c>
       <c r="I19" s="4">
-        <v>0</v>
+        <v>8.4722222222222232</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" s="4">
         <v>0</v>
@@ -1584,21 +1602,79 @@
         <v>0</v>
       </c>
       <c r="D20" s="4">
+        <v>9.5625</v>
+      </c>
+      <c r="E20" s="4">
+        <v>19.576354166666668</v>
+      </c>
+      <c r="F20" s="4">
+        <v>19.576354166666668</v>
+      </c>
+      <c r="G20" s="4">
+        <v>6.4210416666666674</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2.0277777777777781</v>
+      </c>
+      <c r="I20" s="4">
+        <v>8.4722222222222232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="4">
+        <v>4.4247916666666667</v>
+      </c>
+      <c r="C21" s="4">
+        <v>4.4247916666666667</v>
+      </c>
+      <c r="D21" s="4">
+        <v>9.5625</v>
+      </c>
+      <c r="E21" s="4">
+        <v>19.576354166666668</v>
+      </c>
+      <c r="F21" s="4">
+        <v>19.576354166666668</v>
+      </c>
+      <c r="G21" s="4">
+        <v>6.4210416666666674</v>
+      </c>
+      <c r="H21" s="4">
         <v>0</v>
       </c>
-      <c r="E20" s="4">
+      <c r="I21" s="4">
         <v>0</v>
       </c>
-      <c r="F20" s="4">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="4">
         <v>0</v>
       </c>
-      <c r="G20" s="4">
+      <c r="C22" s="4">
         <v>0</v>
       </c>
-      <c r="H20" s="4">
+      <c r="D22" s="4">
         <v>0</v>
       </c>
-      <c r="I20" s="4">
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Precip added to met. new SAL IC.
</commit_message>
<xml_diff>
--- a/matlab/initial_conditions/create_initial_conditions/Defaults_2013_HN.xlsx
+++ b/matlab/initial_conditions/create_initial_conditions/Defaults_2013_HN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Hawkesbury\matlab\initial_conditions\create_initial_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48942DC-A4C2-4B45-8566-57E37209D549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF862F38-E180-493D-92CC-6DA999204399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="4110" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4200" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mean_Initial_Condition" sheetId="1" r:id="rId1"/>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1100,19 +1100,19 @@
         <v>20</v>
       </c>
       <c r="E3" s="1">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F3" s="1">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G3" s="1">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="H3" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="I3" s="5">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>

</xml_diff>